<commit_message>
wip - export dashboard
</commit_message>
<xml_diff>
--- a/storage/templates/dashboard.xlsx
+++ b/storage/templates/dashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hazem/code/cost-control/storage/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{466B5365-0988-D94F-8A07-9E18A4DC41A1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E66AF844-A7E8-E747-953F-BA7602FFA929}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="440" windowWidth="25440" windowHeight="15560" xr2:uid="{5FBE2839-F582-2646-B20D-A87EA405C870}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>AlKifah Contracting Company</t>
   </si>
@@ -73,6 +73,39 @@
   </si>
   <si>
     <t>Time Extension (Days)</t>
+  </si>
+  <si>
+    <t>Budget Information</t>
+  </si>
+  <si>
+    <t>Revision 0</t>
+  </si>
+  <si>
+    <t>Last Revision</t>
+  </si>
+  <si>
+    <t>Total Budget Cost</t>
+  </si>
+  <si>
+    <t>Direct Cost</t>
+  </si>
+  <si>
+    <t>Indirect Cost</t>
+  </si>
+  <si>
+    <t>Management Reserve</t>
+  </si>
+  <si>
+    <t>EAC Contract Amount</t>
+  </si>
+  <si>
+    <t>Planned Profit</t>
+  </si>
+  <si>
+    <t>Planned Profitability</t>
+  </si>
+  <si>
+    <t>Actual Data</t>
   </si>
 </sst>
 </file>
@@ -163,12 +196,73 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -177,7 +271,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -185,34 +279,64 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="40" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="10" fontId="0" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -223,8 +347,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF6CB2EB"/>
       <color rgb="FFBCDEFA"/>
-      <color rgb="FF6CB2EB"/>
       <color rgb="FFDAE1E7"/>
       <color rgb="FF38C172"/>
       <color rgb="FF1F9D55"/>
@@ -542,100 +666,104 @@
   <dimension ref="A1:O32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18:D18"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="10.83203125" customWidth="1"/>
+    <col min="7" max="7" width="13.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:15" ht="24" x14ac:dyDescent="0.2">
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
     </row>
     <row r="8" spans="1:15" ht="21" x14ac:dyDescent="0.2">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
       <c r="J10" s="2"/>
-      <c r="K10" s="6" t="s">
+      <c r="K10" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="L10" s="6"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
       <c r="O10" s="1"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
@@ -654,26 +782,26 @@
       <c r="O11" s="1"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
       <c r="J12" s="2"/>
-      <c r="K12" s="6" t="s">
+      <c r="K12" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="L12" s="6"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
       <c r="O12" s="1"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
@@ -692,22 +820,22 @@
       <c r="O13" s="1"/>
     </row>
     <row r="14" spans="1:15" ht="21" x14ac:dyDescent="0.2">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="8"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
       <c r="O14" s="1"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
@@ -728,26 +856,26 @@
       <c r="O15" s="1"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
       <c r="E16" s="1"/>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G16" s="3"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
       <c r="J16" s="2"/>
-      <c r="K16" s="6" t="s">
+      <c r="K16" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="L16" s="6"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
       <c r="O16" s="1"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
@@ -766,26 +894,26 @@
       <c r="O17" s="1"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="3" t="s">
+      <c r="F18" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G18" s="3"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
       <c r="J18" s="2"/>
-      <c r="K18" s="6" t="s">
+      <c r="K18" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="L18" s="6"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
       <c r="O18" s="1"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
@@ -805,21 +933,23 @@
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
+    <row r="20" spans="1:15" ht="21" x14ac:dyDescent="0.2">
+      <c r="A20" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
       <c r="O20" s="1"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
@@ -839,137 +969,155 @@
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
+      <c r="D22" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
+    <row r="23" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="19"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
+    <row r="24" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="16"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="19"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
+    <row r="25" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="19"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
+    <row r="26" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="19"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
+    <row r="27" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="16"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="19"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
+    <row r="28" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="19"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
+    <row r="29" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="16"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="21"/>
+      <c r="J29" s="21"/>
+      <c r="K29" s="22"/>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
@@ -992,21 +1140,23 @@
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
-      <c r="L31" s="1"/>
-      <c r="M31" s="1"/>
-      <c r="N31" s="1"/>
+    <row r="31" spans="1:15" ht="21" x14ac:dyDescent="0.2">
+      <c r="A31" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="9"/>
+      <c r="M31" s="9"/>
+      <c r="N31" s="9"/>
       <c r="O31" s="1"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
@@ -1027,20 +1177,35 @@
       <c r="O32" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="E6:J6"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H12:I12"/>
+  <mergeCells count="57">
+    <mergeCell ref="H28:K28"/>
+    <mergeCell ref="H29:K29"/>
+    <mergeCell ref="A31:N31"/>
+    <mergeCell ref="H23:K23"/>
+    <mergeCell ref="H24:K24"/>
+    <mergeCell ref="H25:K25"/>
+    <mergeCell ref="H26:K26"/>
+    <mergeCell ref="H27:K27"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="D23:G23"/>
+    <mergeCell ref="D24:G24"/>
+    <mergeCell ref="D25:G25"/>
+    <mergeCell ref="D26:G26"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="D28:G28"/>
+    <mergeCell ref="D29:G29"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="A20:N20"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="H22:K22"/>
     <mergeCell ref="M18:N18"/>
     <mergeCell ref="M12:N12"/>
     <mergeCell ref="M10:N10"/>
@@ -1057,9 +1222,19 @@
     <mergeCell ref="K10:L10"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="C18:D18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="E6:J6"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A5:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>